<commit_message>
merged database layer with latest refactored database from mitch
</commit_message>
<xml_diff>
--- a/formidable-client/assets/opendatakit.collect2/form-files/selects/selects.xlsx
+++ b/formidable-client/assets/opendatakit.collect2/form-files/selects/selects.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="queries" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="survey" state="visible" r:id="rId3"/>
+    <sheet sheetId="2" name="choices" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="queries" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="settings" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62" count="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
   <si>
     <t>comments</t>
   </si>
@@ -22,6 +22,12 @@
     <t>type</t>
   </si>
   <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>inputAttributes.data-type</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -31,6 +37,12 @@
     <t>label</t>
   </si>
   <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
     <t>Cascading select using remote data</t>
   </si>
   <si>
@@ -61,6 +73,9 @@
     <t>select_one birds</t>
   </si>
   <si>
+    <t>grid</t>
+  </si>
+  <si>
     <t>bird</t>
   </si>
   <si>
@@ -85,6 +100,87 @@
     <t>end screen</t>
   </si>
   <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>Choose one:</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>select_one_with_other colors</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>What is your favorite color?</t>
+  </si>
+  <si>
+    <t>selected function with arguement not included in choices.</t>
+  </si>
+  <si>
+    <t>selected(data('color'), 'teal')</t>
+  </si>
+  <si>
+    <t>Teal is a good choice.</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>h_select</t>
+  </si>
+  <si>
+    <t>Horizontal select example.</t>
+  </si>
+  <si>
+    <t>select_one regions_csv</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Choose a region:</t>
+  </si>
+  <si>
+    <t>select_one countries_csv</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Choose a country:</t>
+  </si>
+  <si>
+    <t>context.region === data('region')</t>
+  </si>
+  <si>
+    <t>select_one content_provider_test</t>
+  </si>
+  <si>
+    <t>cp_test</t>
+  </si>
+  <si>
+    <t>This demos a content provider query.</t>
+  </si>
+  <si>
+    <t>You will need to install a content provider app for the query to work. There is an example app available here: https://github.com/nathanathan/FileContentProviderExample</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -148,16 +244,46 @@
     <t>media/jay.png</t>
   </si>
   <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
     <t>uri</t>
   </si>
   <si>
     <t>callback</t>
-  </si>
-  <si>
-    <t>param.format</t>
-  </si>
-  <si>
-    <t>param.q</t>
   </si>
   <si>
     <t>states</t>
@@ -178,10 +304,34 @@
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('state') + "'")</t>
   </si>
   <si>
-    <t>odk_values</t>
-  </si>
-  <si>
-    <t>odkquery://table_id/elementKey1/elementKey5/?selection=encodeURIComponent('elementKey2=? and elementKey3&gt;5')&amp;selectionArgs=encodeURIComponent(JSON.stringify([data('state')])</t>
+    <t>regions_csv</t>
+  </si>
+  <si>
+    <t>"regions.csv"</t>
+  </si>
+  <si>
+    <t>_.chain(context).pluck('region').uniq().map(function(region){
+return {name:region, label:region};
+}).value()</t>
+  </si>
+  <si>
+    <t>countries_csv</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){
+place.name = place.country;
+place.label = place.country;
+return place;
+})</t>
+  </si>
+  <si>
+    <t>content_provider_test</t>
+  </si>
+  <si>
+    <t>"content://org.opendatakit.FileContentProviderExample/"</t>
+  </si>
+  <si>
+    <t>[context]</t>
   </si>
   <si>
     <t>setting</t>
@@ -190,16 +340,16 @@
     <t>value</t>
   </si>
   <si>
-    <t>formId</t>
+    <t>form_id</t>
   </si>
   <si>
     <t>selects</t>
   </si>
   <si>
-    <t>formVersion</t>
-  </si>
-  <si>
-    <t>formTitle</t>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>form_title</t>
   </si>
   <si>
     <t>Select Examples</t>
@@ -354,50 +504,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" xfId="0" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="2" fillId="2" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="3" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="4" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="4" fillId="5" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="6" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="7" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="8" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="5" fillId="9" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="10" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="6" fillId="11" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="10" borderId="0" fontId="0" applyNumberFormat="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,13 +561,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="34.29"/>
-    <col max="2" min="2" customWidth="1" width="35.0"/>
-    <col max="3" min="3" customWidth="1" width="38.71"/>
-    <col max="4" min="4" customWidth="1" width="32.71"/>
-    <col max="5" min="5" customWidth="1" width="37.71"/>
+    <col min="1" customWidth="1" max="1" width="34.29"/>
+    <col min="2" customWidth="1" max="2" width="35.0"/>
+    <col min="4" customWidth="1" max="4" width="20.71"/>
+    <col min="5" customWidth="1" max="5" width="38.71"/>
+    <col min="6" customWidth="1" max="6" width="32.71"/>
+    <col min="7" customWidth="1" max="7" width="46.0"/>
+    <col min="9" customWidth="1" max="9" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -436,115 +588,240 @@
       <c t="s" r="E1">
         <v>4</v>
       </c>
+      <c t="s" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" r="I1">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="12" r="A2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c t="s" r="B2">
-        <v>6</v>
-      </c>
-      <c t="s" r="D2">
-        <v>7</v>
-      </c>
-      <c t="s" r="E2">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c t="s" r="F2">
+        <v>11</v>
+      </c>
+      <c t="s" r="G2">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c s="12" r="A3"/>
       <c t="s" r="B3">
-        <v>9</v>
-      </c>
-      <c t="s" r="D3">
-        <v>10</v>
-      </c>
-      <c t="s" r="E3">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c t="s" r="F3">
+        <v>14</v>
+      </c>
+      <c t="s" r="G3">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="12" r="A4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c t="s" r="B4">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c s="12" r="A5"/>
       <c t="s" r="B5">
-        <v>14</v>
-      </c>
-      <c t="s" r="D5">
-        <v>15</v>
-      </c>
-      <c t="s" r="E5">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c t="s" r="C5">
+        <v>19</v>
+      </c>
+      <c t="s" r="F5">
+        <v>20</v>
+      </c>
+      <c t="s" r="G5">
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c s="12" r="A6"/>
       <c t="s" r="B6">
-        <v>17</v>
-      </c>
-      <c t="s" r="C6">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c t="s" r="E6">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="G6">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c s="12" r="A7"/>
       <c t="s" r="B7">
-        <v>17</v>
-      </c>
-      <c t="s" r="C7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c t="s" r="E7">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c t="s" r="G7">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c s="12" r="A8"/>
       <c t="s" r="B8">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c s="12" r="A9"/>
+      <c t="s" r="B9">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
       <c s="12" r="A10"/>
+      <c t="s" r="B10">
+        <v>28</v>
+      </c>
+      <c t="s" r="C10">
+        <v>29</v>
+      </c>
+      <c t="s" r="F10">
+        <v>30</v>
+      </c>
+      <c t="s" r="G10">
+        <v>31</v>
+      </c>
     </row>
     <row r="11">
       <c s="12" r="A11"/>
+      <c t="s" r="B11">
+        <v>28</v>
+      </c>
+      <c t="s" r="C11">
+        <v>29</v>
+      </c>
+      <c t="s" r="F11">
+        <v>32</v>
+      </c>
+      <c t="s" r="G11">
+        <v>31</v>
+      </c>
     </row>
     <row r="12">
       <c s="12" r="A12"/>
+      <c t="s" r="B12">
+        <v>28</v>
+      </c>
+      <c t="s" r="C12">
+        <v>29</v>
+      </c>
+      <c t="s" r="F12">
+        <v>33</v>
+      </c>
+      <c t="s" r="G12">
+        <v>31</v>
+      </c>
     </row>
     <row r="13">
       <c s="12" r="A13"/>
+      <c t="s" r="B13">
+        <v>27</v>
+      </c>
     </row>
     <row r="14">
       <c s="12" r="A14"/>
+      <c t="s" r="B14">
+        <v>34</v>
+      </c>
+      <c t="s" r="F14">
+        <v>35</v>
+      </c>
+      <c t="s" r="G14">
+        <v>36</v>
+      </c>
     </row>
     <row r="15">
-      <c s="12" r="A15"/>
+      <c t="s" s="12" r="A15">
+        <v>37</v>
+      </c>
+      <c t="s" r="B15">
+        <v>22</v>
+      </c>
+      <c t="s" r="E15">
+        <v>38</v>
+      </c>
+      <c t="s" r="G15">
+        <v>39</v>
+      </c>
     </row>
     <row r="16">
       <c s="12" r="A16"/>
+      <c t="s" r="B16">
+        <v>28</v>
+      </c>
+      <c t="s" r="D16">
+        <v>40</v>
+      </c>
+      <c t="s" r="F16">
+        <v>41</v>
+      </c>
+      <c t="s" r="G16">
+        <v>42</v>
+      </c>
     </row>
     <row r="17">
       <c s="12" r="A17"/>
+      <c t="s" r="B17">
+        <v>43</v>
+      </c>
+      <c t="s" r="F17">
+        <v>44</v>
+      </c>
+      <c t="s" r="G17">
+        <v>45</v>
+      </c>
     </row>
     <row r="18">
       <c s="12" r="A18"/>
+      <c t="s" r="B18">
+        <v>46</v>
+      </c>
+      <c t="s" r="C18">
+        <v>47</v>
+      </c>
+      <c t="s" r="F18">
+        <v>48</v>
+      </c>
+      <c t="s" r="G18">
+        <v>49</v>
+      </c>
+      <c t="s" r="I18">
+        <v>50</v>
+      </c>
     </row>
     <row r="19">
       <c s="12" r="A19"/>
+      <c t="s" r="B19">
+        <v>51</v>
+      </c>
+      <c t="s" r="F19">
+        <v>52</v>
+      </c>
+      <c t="s" r="G19">
+        <v>53</v>
+      </c>
+      <c t="s" r="H19">
+        <v>54</v>
+      </c>
     </row>
     <row r="20">
       <c s="12" r="A20"/>
@@ -557,6 +834,12 @@
     </row>
     <row r="23">
       <c s="12" r="A23"/>
+    </row>
+    <row r="24">
+      <c s="12" r="A24"/>
+    </row>
+    <row r="25">
+      <c s="12" r="A25"/>
     </row>
   </sheetData>
 </worksheet>
@@ -567,116 +850,174 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c t="s" r="B1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c t="s" r="C1">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c t="s" r="D1">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B2">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c t="s" r="C2">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B3">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c t="s" r="C3">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B4">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c t="s" r="C4">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B5">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c t="s" r="C5">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B6">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c t="s" r="C6">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B7">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c t="s" r="C7">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B8">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c t="s" r="C8">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B9">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c t="s" r="C9">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B10">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c t="s" r="C10">
-        <v>43</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>76</v>
+      </c>
+      <c t="s" r="B12">
+        <v>77</v>
+      </c>
+      <c t="s" r="D12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" r="A13">
+        <v>76</v>
+      </c>
+      <c t="s" r="B13">
+        <v>79</v>
+      </c>
+      <c t="s" r="D13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" r="A15">
+        <v>81</v>
+      </c>
+      <c t="s" r="B15">
+        <v>82</v>
+      </c>
+      <c t="s" r="D15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" r="A16">
+        <v>81</v>
+      </c>
+      <c t="s" r="B16">
+        <v>84</v>
+      </c>
+      <c t="s" r="D16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" r="A17">
+        <v>81</v>
+      </c>
+      <c t="s" r="B17">
+        <v>86</v>
+      </c>
+      <c t="s" r="D17">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -688,57 +1029,76 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="39.14"/>
-    <col max="3" min="3" customWidth="1" width="35.14"/>
+    <col min="2" customWidth="1" max="2" width="71.29"/>
+    <col min="3" customWidth="1" max="3" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c t="s" r="B1">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c t="s" r="C1">
-        <v>45</v>
-      </c>
-      <c t="s" r="D1">
-        <v>46</v>
-      </c>
-      <c t="s" r="E1">
-        <v>47</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c t="s" r="B2">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c t="s" r="C2">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c t="s" r="B3">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c t="s" r="C3">
-        <v>50</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" r="A4">
+        <v>95</v>
+      </c>
+      <c t="s" r="B4">
+        <v>96</v>
+      </c>
+      <c t="s" r="C4">
+        <v>97</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c t="s" r="B5">
-        <v>54</v>
+        <v>96</v>
+      </c>
+      <c t="s" r="C5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6">
+        <v>100</v>
+      </c>
+      <c t="s" r="B6">
+        <v>101</v>
+      </c>
+      <c t="s" r="C6">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -750,29 +1110,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -780,10 +1140,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c t="s" r="B4">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
merged with database refactoring from Mitch
</commit_message>
<xml_diff>
--- a/formidable-client/assets/opendatakit.collect2/form-files/selects/selects.xlsx
+++ b/formidable-client/assets/opendatakit.collect2/form-files/selects/selects.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="queries" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="survey" state="visible" r:id="rId3"/>
+    <sheet sheetId="2" name="choices" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="queries" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="settings" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62" count="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="110">
   <si>
     <t>comments</t>
   </si>
@@ -22,6 +22,12 @@
     <t>type</t>
   </si>
   <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>inputAttributes.data-type</t>
+  </si>
+  <si>
     <t>condition</t>
   </si>
   <si>
@@ -31,6 +37,12 @@
     <t>label</t>
   </si>
   <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
     <t>Cascading select using remote data</t>
   </si>
   <si>
@@ -61,6 +73,9 @@
     <t>select_one birds</t>
   </si>
   <si>
+    <t>grid</t>
+  </si>
+  <si>
     <t>bird</t>
   </si>
   <si>
@@ -85,6 +100,87 @@
     <t>end screen</t>
   </si>
   <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>Choose one:</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>select_one_with_other colors</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>What is your favorite color?</t>
+  </si>
+  <si>
+    <t>selected function with arguement not included in choices.</t>
+  </si>
+  <si>
+    <t>selected(data('color'), 'teal')</t>
+  </si>
+  <si>
+    <t>Teal is a good choice.</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>h_select</t>
+  </si>
+  <si>
+    <t>Horizontal select example.</t>
+  </si>
+  <si>
+    <t>select_one regions_csv</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Choose a region:</t>
+  </si>
+  <si>
+    <t>select_one countries_csv</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Choose a country:</t>
+  </si>
+  <si>
+    <t>context.region === data('region')</t>
+  </si>
+  <si>
+    <t>select_one content_provider_test</t>
+  </si>
+  <si>
+    <t>cp_test</t>
+  </si>
+  <si>
+    <t>This demos a content provider query.</t>
+  </si>
+  <si>
+    <t>You will need to install a content provider app for the query to work. There is an example app available here: https://github.com/nathanathan/FileContentProviderExample</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -148,16 +244,46 @@
     <t>media/jay.png</t>
   </si>
   <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
     <t>uri</t>
   </si>
   <si>
     <t>callback</t>
-  </si>
-  <si>
-    <t>param.format</t>
-  </si>
-  <si>
-    <t>param.q</t>
   </si>
   <si>
     <t>states</t>
@@ -178,10 +304,34 @@
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('state') + "'")</t>
   </si>
   <si>
-    <t>odk_values</t>
-  </si>
-  <si>
-    <t>odkquery://table_id/elementKey1/elementKey5/?selection=encodeURIComponent('elementKey2=? and elementKey3&gt;5')&amp;selectionArgs=encodeURIComponent(JSON.stringify([data('state')])</t>
+    <t>regions_csv</t>
+  </si>
+  <si>
+    <t>"regions.csv"</t>
+  </si>
+  <si>
+    <t>_.chain(context).pluck('region').uniq().map(function(region){
+return {name:region, label:region};
+}).value()</t>
+  </si>
+  <si>
+    <t>countries_csv</t>
+  </si>
+  <si>
+    <t>_.map(context, function(place){
+place.name = place.country;
+place.label = place.country;
+return place;
+})</t>
+  </si>
+  <si>
+    <t>content_provider_test</t>
+  </si>
+  <si>
+    <t>"content://org.opendatakit.FileContentProviderExample/"</t>
+  </si>
+  <si>
+    <t>[context]</t>
   </si>
   <si>
     <t>setting</t>
@@ -190,16 +340,16 @@
     <t>value</t>
   </si>
   <si>
-    <t>formId</t>
+    <t>form_id</t>
   </si>
   <si>
     <t>selects</t>
   </si>
   <si>
-    <t>formVersion</t>
-  </si>
-  <si>
-    <t>formTitle</t>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>form_title</t>
   </si>
   <si>
     <t>Select Examples</t>
@@ -354,50 +504,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" xfId="0" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="2" fillId="2" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="3" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="4" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="4" fillId="5" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="6" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="7" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="8" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="5" fillId="9" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="10" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="6" fillId="11" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="10" borderId="0" fontId="0" applyNumberFormat="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4" applyFill="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="11" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,13 +561,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="34.29"/>
-    <col max="2" min="2" customWidth="1" width="35.0"/>
-    <col max="3" min="3" customWidth="1" width="38.71"/>
-    <col max="4" min="4" customWidth="1" width="32.71"/>
-    <col max="5" min="5" customWidth="1" width="37.71"/>
+    <col min="1" customWidth="1" max="1" width="34.29"/>
+    <col min="2" customWidth="1" max="2" width="35.0"/>
+    <col min="4" customWidth="1" max="4" width="20.71"/>
+    <col min="5" customWidth="1" max="5" width="38.71"/>
+    <col min="6" customWidth="1" max="6" width="32.71"/>
+    <col min="7" customWidth="1" max="7" width="46.0"/>
+    <col min="9" customWidth="1" max="9" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -436,115 +588,240 @@
       <c t="s" r="E1">
         <v>4</v>
       </c>
+      <c t="s" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" r="I1">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="12" r="A2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c t="s" r="B2">
-        <v>6</v>
-      </c>
-      <c t="s" r="D2">
-        <v>7</v>
-      </c>
-      <c t="s" r="E2">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c t="s" r="F2">
+        <v>11</v>
+      </c>
+      <c t="s" r="G2">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c s="12" r="A3"/>
       <c t="s" r="B3">
-        <v>9</v>
-      </c>
-      <c t="s" r="D3">
-        <v>10</v>
-      </c>
-      <c t="s" r="E3">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c t="s" r="F3">
+        <v>14</v>
+      </c>
+      <c t="s" r="G3">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="12" r="A4">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c t="s" r="B4">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c s="12" r="A5"/>
       <c t="s" r="B5">
-        <v>14</v>
-      </c>
-      <c t="s" r="D5">
-        <v>15</v>
-      </c>
-      <c t="s" r="E5">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c t="s" r="C5">
+        <v>19</v>
+      </c>
+      <c t="s" r="F5">
+        <v>20</v>
+      </c>
+      <c t="s" r="G5">
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c s="12" r="A6"/>
       <c t="s" r="B6">
-        <v>17</v>
-      </c>
-      <c t="s" r="C6">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c t="s" r="E6">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c t="s" r="G6">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c s="12" r="A7"/>
       <c t="s" r="B7">
-        <v>17</v>
-      </c>
-      <c t="s" r="C7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c t="s" r="E7">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c t="s" r="G7">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c s="12" r="A8"/>
       <c t="s" r="B8">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c s="12" r="A9"/>
+      <c t="s" r="B9">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
       <c s="12" r="A10"/>
+      <c t="s" r="B10">
+        <v>28</v>
+      </c>
+      <c t="s" r="C10">
+        <v>29</v>
+      </c>
+      <c t="s" r="F10">
+        <v>30</v>
+      </c>
+      <c t="s" r="G10">
+        <v>31</v>
+      </c>
     </row>
     <row r="11">
       <c s="12" r="A11"/>
+      <c t="s" r="B11">
+        <v>28</v>
+      </c>
+      <c t="s" r="C11">
+        <v>29</v>
+      </c>
+      <c t="s" r="F11">
+        <v>32</v>
+      </c>
+      <c t="s" r="G11">
+        <v>31</v>
+      </c>
     </row>
     <row r="12">
       <c s="12" r="A12"/>
+      <c t="s" r="B12">
+        <v>28</v>
+      </c>
+      <c t="s" r="C12">
+        <v>29</v>
+      </c>
+      <c t="s" r="F12">
+        <v>33</v>
+      </c>
+      <c t="s" r="G12">
+        <v>31</v>
+      </c>
     </row>
     <row r="13">
       <c s="12" r="A13"/>
+      <c t="s" r="B13">
+        <v>27</v>
+      </c>
     </row>
     <row r="14">
       <c s="12" r="A14"/>
+      <c t="s" r="B14">
+        <v>34</v>
+      </c>
+      <c t="s" r="F14">
+        <v>35</v>
+      </c>
+      <c t="s" r="G14">
+        <v>36</v>
+      </c>
     </row>
     <row r="15">
-      <c s="12" r="A15"/>
+      <c t="s" s="12" r="A15">
+        <v>37</v>
+      </c>
+      <c t="s" r="B15">
+        <v>22</v>
+      </c>
+      <c t="s" r="E15">
+        <v>38</v>
+      </c>
+      <c t="s" r="G15">
+        <v>39</v>
+      </c>
     </row>
     <row r="16">
       <c s="12" r="A16"/>
+      <c t="s" r="B16">
+        <v>28</v>
+      </c>
+      <c t="s" r="D16">
+        <v>40</v>
+      </c>
+      <c t="s" r="F16">
+        <v>41</v>
+      </c>
+      <c t="s" r="G16">
+        <v>42</v>
+      </c>
     </row>
     <row r="17">
       <c s="12" r="A17"/>
+      <c t="s" r="B17">
+        <v>43</v>
+      </c>
+      <c t="s" r="F17">
+        <v>44</v>
+      </c>
+      <c t="s" r="G17">
+        <v>45</v>
+      </c>
     </row>
     <row r="18">
       <c s="12" r="A18"/>
+      <c t="s" r="B18">
+        <v>46</v>
+      </c>
+      <c t="s" r="C18">
+        <v>47</v>
+      </c>
+      <c t="s" r="F18">
+        <v>48</v>
+      </c>
+      <c t="s" r="G18">
+        <v>49</v>
+      </c>
+      <c t="s" r="I18">
+        <v>50</v>
+      </c>
     </row>
     <row r="19">
       <c s="12" r="A19"/>
+      <c t="s" r="B19">
+        <v>51</v>
+      </c>
+      <c t="s" r="F19">
+        <v>52</v>
+      </c>
+      <c t="s" r="G19">
+        <v>53</v>
+      </c>
+      <c t="s" r="H19">
+        <v>54</v>
+      </c>
     </row>
     <row r="20">
       <c s="12" r="A20"/>
@@ -557,6 +834,12 @@
     </row>
     <row r="23">
       <c s="12" r="A23"/>
+    </row>
+    <row r="24">
+      <c s="12" r="A24"/>
+    </row>
+    <row r="25">
+      <c s="12" r="A25"/>
     </row>
   </sheetData>
 </worksheet>
@@ -567,116 +850,174 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c t="s" r="B1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c t="s" r="C1">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c t="s" r="D1">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B2">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c t="s" r="C2">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B3">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c t="s" r="C3">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B4">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c t="s" r="C4">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B5">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c t="s" r="C5">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B6">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c t="s" r="C6">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B7">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c t="s" r="C7">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B8">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c t="s" r="C8">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B9">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c t="s" r="C9">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c t="s" r="B10">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c t="s" r="C10">
-        <v>43</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>76</v>
+      </c>
+      <c t="s" r="B12">
+        <v>77</v>
+      </c>
+      <c t="s" r="D12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" r="A13">
+        <v>76</v>
+      </c>
+      <c t="s" r="B13">
+        <v>79</v>
+      </c>
+      <c t="s" r="D13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" r="A15">
+        <v>81</v>
+      </c>
+      <c t="s" r="B15">
+        <v>82</v>
+      </c>
+      <c t="s" r="D15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" r="A16">
+        <v>81</v>
+      </c>
+      <c t="s" r="B16">
+        <v>84</v>
+      </c>
+      <c t="s" r="D16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" r="A17">
+        <v>81</v>
+      </c>
+      <c t="s" r="B17">
+        <v>86</v>
+      </c>
+      <c t="s" r="D17">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -688,57 +1029,76 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="39.14"/>
-    <col max="3" min="3" customWidth="1" width="35.14"/>
+    <col min="2" customWidth="1" max="2" width="71.29"/>
+    <col min="3" customWidth="1" max="3" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c t="s" r="B1">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c t="s" r="C1">
-        <v>45</v>
-      </c>
-      <c t="s" r="D1">
-        <v>46</v>
-      </c>
-      <c t="s" r="E1">
-        <v>47</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c t="s" r="B2">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c t="s" r="C2">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c t="s" r="B3">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c t="s" r="C3">
-        <v>50</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" r="A4">
+        <v>95</v>
+      </c>
+      <c t="s" r="B4">
+        <v>96</v>
+      </c>
+      <c t="s" r="C4">
+        <v>97</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c t="s" r="B5">
-        <v>54</v>
+        <v>96</v>
+      </c>
+      <c t="s" r="C5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6">
+        <v>100</v>
+      </c>
+      <c t="s" r="B6">
+        <v>101</v>
+      </c>
+      <c t="s" r="C6">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -750,29 +1110,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="17.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c s="2" r="C1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c s="2" r="C2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -780,10 +1140,10 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c t="s" r="B4">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">

</xml_diff>